<commit_message>
Fix Date in import
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -41,9 +41,6 @@
     <t>PURCHASE REQUEST</t>
   </si>
   <si>
-    <t>(Y-m-d)</t>
-  </si>
-  <si>
     <t xml:space="preserve">       Requestor:</t>
   </si>
   <si>
@@ -89,10 +86,25 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
-    <t>Test PR</t>
-  </si>
-  <si>
-    <t>PR123</t>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Test Item</t>
+  </si>
+  <si>
+    <t>Test Item 2</t>
+  </si>
+  <si>
+    <t>Purchase Test</t>
+  </si>
+  <si>
+    <t>IT Department</t>
+  </si>
+  <si>
+    <t>PR11111</t>
   </si>
   <si>
     <t>Test Purpose</t>
@@ -101,55 +113,25 @@
     <t>DG1</t>
   </si>
   <si>
-    <t>Test Department</t>
-  </si>
-  <si>
-    <t>Test Requestor</t>
-  </si>
-  <si>
-    <t>pcs</t>
-  </si>
-  <si>
-    <t>Lumber, Coco, 2" x 3" x 12ft</t>
-  </si>
-  <si>
-    <t>Lumber, Coco, 2" x 2" x 12ft</t>
-  </si>
-  <si>
-    <t>Plywood, Ordinary, 4ft x 8ft x 1/4"</t>
-  </si>
-  <si>
-    <t>Plywood, Ordinary, 4ft x 8ft x 3/4"</t>
-  </si>
-  <si>
-    <t>Nails, Common 4"</t>
-  </si>
-  <si>
-    <t>Nails, Common 2-1/2"</t>
-  </si>
-  <si>
-    <t>roll/s</t>
-  </si>
-  <si>
-    <t>bottle/s</t>
-  </si>
-  <si>
-    <t>set/s</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>Hinges, 3" x 3"</t>
-  </si>
-  <si>
-    <t>Handle, Door</t>
-  </si>
-  <si>
-    <t>Hasp, Safety, 5"</t>
+    <t>Stephine Severino</t>
+  </si>
+  <si>
+    <t>Test Item 3</t>
+  </si>
+  <si>
+    <t>Test Item 4</t>
+  </si>
+  <si>
+    <t>Test Item 5</t>
+  </si>
+  <si>
+    <t>Test Item 6</t>
+  </si>
+  <si>
+    <t>Test Item 7</t>
+  </si>
+  <si>
+    <t>Test Item 8</t>
   </si>
 </sst>
 </file>
@@ -191,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,18 +317,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,6 +331,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -356,30 +345,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -391,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -403,13 +401,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -418,6 +416,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF428A2E"/>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -427,6 +431,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="381000"/>
+          <a:ext cx="1200150" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,450 +748,456 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J21" sqref="J21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="C2" s="33" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="K2" s="5"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="34" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="K3" s="6"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="6"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="29" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="7"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="32"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="H7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="H7" s="8" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="16">
+        <v>43642</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="H8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="H9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="27">
+        <v>1</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="15">
-        <v>43642</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="H8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="H9" s="8" t="s">
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="17">
-        <v>1</v>
-      </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="18"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="17" t="s">
+      <c r="D14" s="5">
+        <v>123</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="18"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="21"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" s="11">
-        <v>32</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="11">
-        <v>123</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>28</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="15">
-        <v>43645</v>
-      </c>
-      <c r="K14" s="16"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="16">
+        <v>43642</v>
+      </c>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="11">
-        <v>46</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="3">
-        <v>12123</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>29</v>
+      <c r="B15" s="5">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5">
+        <v>44555</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="15">
-        <v>43646</v>
-      </c>
-      <c r="K15" s="16"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="16">
+        <v>43643</v>
+      </c>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="11">
-        <v>31</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3">
-        <v>12343</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>30</v>
+      <c r="B16" s="5">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="5">
+        <v>123</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="15">
-        <v>43647</v>
-      </c>
-      <c r="K16" s="16"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="16">
+        <v>43644</v>
+      </c>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B17" s="11">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3443</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>31</v>
+      <c r="B17" s="5">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5">
+        <v>45342</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="15">
-        <v>43648</v>
-      </c>
-      <c r="K17" s="16"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="16">
+        <v>43645</v>
+      </c>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>5</v>
       </c>
-      <c r="B18" s="11">
-        <v>8</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="3">
-        <v>342</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>32</v>
+      <c r="B18" s="5">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="5">
+        <v>123451</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="15">
-        <v>43649</v>
-      </c>
-      <c r="K18" s="16"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="16">
+        <v>43646</v>
+      </c>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="B19" s="11">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="3">
-        <v>234</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>33</v>
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="5">
+        <v>345521</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="15">
-        <v>43650</v>
-      </c>
-      <c r="K19" s="16"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="16">
+        <v>43647</v>
+      </c>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>7</v>
       </c>
-      <c r="B20" s="3">
-        <v>4</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1234324</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>39</v>
+      <c r="B20" s="5">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="5">
+        <v>54234</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="15">
-        <v>43651</v>
-      </c>
-      <c r="K20" s="16"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="16">
+        <v>43648</v>
+      </c>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>8</v>
       </c>
-      <c r="B21" s="3">
-        <v>10</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="3">
-        <v>213234</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>40</v>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4521321</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="15">
-        <v>43652</v>
-      </c>
-      <c r="K21" s="16"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="16">
+        <v>43649</v>
+      </c>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>9</v>
       </c>
-      <c r="B22" s="3">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="3">
-        <v>234234</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>41</v>
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="5">
+        <v>425342</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="15">
-        <v>43653</v>
-      </c>
-      <c r="K22" s="16"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="16">
+        <v>43650</v>
+      </c>
+      <c r="K22" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="38">
@@ -1155,7 +1214,6 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E17:I17"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="I8:K8"/>
@@ -1163,16 +1221,17 @@
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:I13"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
     <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="J21:K21"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="E18:I18"/>
@@ -1183,5 +1242,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Due date approved by noted by sa Groupings
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CENPRI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10367008-857F-4CAC-A8E1-D93003E101BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,40 +86,40 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>unit/s</t>
-  </si>
-  <si>
     <t>Bacolod</t>
   </si>
   <si>
-    <t>Jonah</t>
-  </si>
-  <si>
-    <t>pr2019-1001</t>
-  </si>
-  <si>
-    <t>Test Purpose</t>
-  </si>
-  <si>
-    <t>Test Enduse</t>
-  </si>
-  <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>Keyboard</t>
-  </si>
-  <si>
-    <t>Speakers</t>
+    <t>PR-2948-2984</t>
+  </si>
+  <si>
+    <t>Stator</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>IT Department</t>
+  </si>
+  <si>
+    <t>Lumber</t>
+  </si>
+  <si>
+    <t>Nails</t>
+  </si>
+  <si>
+    <t>Hasp</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>Stephine David Severino</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -321,6 +320,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -345,40 +356,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -433,13 +432,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -733,11 +726,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,14 +756,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="11"/>
@@ -778,14 +771,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="12"/>
@@ -793,14 +786,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="12"/>
@@ -808,98 +801,98 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
       <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="28"/>
+      <c r="I7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="20">
-        <v>43656</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="24">
+        <v>43642</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
       <c r="H8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="28"/>
+      <c r="I8" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="H9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="22">
-        <v>2</v>
-      </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="28"/>
+      <c r="I9" s="26">
+        <v>1</v>
+      </c>
+      <c r="J9" s="27"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="8"/>
@@ -909,34 +902,34 @@
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="28"/>
+      <c r="C11" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
+      <c r="C12" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -951,17 +944,17 @@
       <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="29" t="s">
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="30"/>
+      <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -971,17 +964,21 @@
         <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="D14" s="5">
+        <v>12111</v>
+      </c>
       <c r="E14" s="36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="20"/>
+      <c r="J14" s="24">
+        <v>43502</v>
+      </c>
       <c r="K14" s="39"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -989,20 +986,24 @@
         <v>2</v>
       </c>
       <c r="B15" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1222</v>
+      </c>
       <c r="E15" s="36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="38"/>
-      <c r="J15" s="20"/>
+      <c r="J15" s="24">
+        <v>43512</v>
+      </c>
       <c r="K15" s="39"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1010,50 +1011,54 @@
         <v>3</v>
       </c>
       <c r="B16" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1233</v>
+      </c>
       <c r="E16" s="36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="38"/>
-      <c r="J16" s="20"/>
+      <c r="J16" s="24">
+        <v>43514</v>
+      </c>
       <c r="K16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:I13"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="C7:E7"/>
     <mergeCell ref="I9:K9"/>
-    <mergeCell ref="J13:K13"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add Due Date, Noted By, Approved By In Pr Group
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">       Requestor:</t>
   </si>
   <si>
-    <t xml:space="preserve">  Deptartment:</t>
-  </si>
-  <si>
     <t>Item No.</t>
   </si>
   <si>
@@ -86,34 +83,46 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>PR-2948-2984</t>
-  </si>
-  <si>
-    <t>Stator</t>
-  </si>
-  <si>
-    <t>Warehouse</t>
+    <t xml:space="preserve">  Department:</t>
+  </si>
+  <si>
+    <t>Test Purchase</t>
+  </si>
+  <si>
+    <t>PR2019-07-09</t>
+  </si>
+  <si>
+    <t>Test Purpose</t>
+  </si>
+  <si>
+    <t>Test Enduse</t>
   </si>
   <si>
     <t>IT Department</t>
   </si>
   <si>
-    <t>Lumber</t>
-  </si>
-  <si>
-    <t>Nails</t>
-  </si>
-  <si>
-    <t>Hasp</t>
-  </si>
-  <si>
-    <t>kg/s</t>
-  </si>
-  <si>
-    <t>Stephine David Severino</t>
+    <t>Stephine</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Test Screw</t>
+  </si>
+  <si>
+    <t>Test Hammer</t>
+  </si>
+  <si>
+    <t>Test Ballpen</t>
+  </si>
+  <si>
+    <t>Test Pencil</t>
+  </si>
+  <si>
+    <t>Test Paper</t>
+  </si>
+  <si>
+    <t>Test Monitor</t>
   </si>
 </sst>
 </file>
@@ -320,66 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -389,7 +338,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -727,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,14 +765,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="11"/>
@@ -771,14 +780,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="12"/>
@@ -786,14 +795,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="12"/>
@@ -801,98 +810,98 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="H7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="29"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="24">
-        <v>43642</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="19">
+        <v>43655</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
       <c r="H8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="27"/>
+      <c r="I8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="28"/>
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="27">
+        <v>2</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="H9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="26">
-        <v>1</v>
-      </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="29"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="8"/>
@@ -900,111 +909,107 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="28"/>
       <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5">
-        <v>12111</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="24">
-        <v>43502</v>
-      </c>
-      <c r="K14" s="39"/>
+        <v>124</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
       <c r="B15" s="5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5">
+        <v>12354</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="5">
-        <v>1222</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="24">
-        <v>43512</v>
-      </c>
-      <c r="K15" s="39"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1014,25 +1019,110 @@
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5">
-        <v>1233</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="24">
-        <v>43514</v>
-      </c>
-      <c r="K16" s="39"/>
+        <v>1312354</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="5">
+        <v>32146</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="5">
+        <v>234</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="5">
+        <v>36</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="32">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="E14:I14"/>
@@ -1041,24 +1131,12 @@
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ADD Cancel Function PO
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -86,7 +86,43 @@
     <t xml:space="preserve">  Department:</t>
   </si>
   <si>
-    <t>(Y-m-d)</t>
+    <t>Test Purchase</t>
+  </si>
+  <si>
+    <t>PR2019-07-09</t>
+  </si>
+  <si>
+    <t>Test Purpose</t>
+  </si>
+  <si>
+    <t>Test Enduse</t>
+  </si>
+  <si>
+    <t>IT Department</t>
+  </si>
+  <si>
+    <t>Stephine</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Test Screw</t>
+  </si>
+  <si>
+    <t>Test Hammer</t>
+  </si>
+  <si>
+    <t>Test Ballpen</t>
+  </si>
+  <si>
+    <t>Test Pencil</t>
+  </si>
+  <si>
+    <t>Test Paper</t>
+  </si>
+  <si>
+    <t>Test Monitor</t>
   </si>
 </sst>
 </file>
@@ -272,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -293,16 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -710,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:K19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,14 +765,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="11"/>
@@ -754,14 +780,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="12"/>
@@ -769,14 +795,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="12"/>
@@ -784,90 +810,98 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="40"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
+      <c r="I7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="19">
+        <v>43655</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
       <c r="H8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
+      <c r="I8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
       <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
+      <c r="I9" s="27">
+        <v>2</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="8"/>
@@ -877,30 +911,34 @@
       <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
+      <c r="C11" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30"/>
+      <c r="C12" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -915,220 +953,155 @@
       <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="25" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="26"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="B14" s="5">
-        <v>213</v>
-      </c>
-      <c r="C14" s="5">
-        <v>2314</v>
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="5">
-        <v>2134</v>
-      </c>
-      <c r="E14" s="20">
-        <v>234</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
+        <v>124</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="B15" s="5">
-        <v>123</v>
-      </c>
-      <c r="C15" s="5">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="5">
-        <v>34</v>
-      </c>
-      <c r="E15" s="20">
-        <v>234</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
+        <v>12354</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>213</v>
+        <v>3</v>
       </c>
       <c r="B16" s="5">
-        <v>213</v>
-      </c>
-      <c r="C16" s="5">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D16" s="5">
-        <v>234</v>
-      </c>
-      <c r="E16" s="20">
-        <v>324</v>
-      </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="24"/>
+        <v>1312354</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>213</v>
+        <v>4</v>
       </c>
       <c r="B17" s="5">
-        <v>213</v>
-      </c>
-      <c r="C17" s="5">
-        <v>324</v>
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="5">
-        <v>2134</v>
-      </c>
-      <c r="E17" s="20">
-        <v>234</v>
-      </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="24"/>
+        <v>32146</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="B18" s="5">
-        <v>23</v>
-      </c>
-      <c r="C18" s="5">
-        <v>2314</v>
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D18" s="5">
         <v>234</v>
       </c>
-      <c r="E18" s="20">
-        <v>234</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="E18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>213</v>
+        <v>6</v>
       </c>
       <c r="B19" s="5">
-        <v>213</v>
-      </c>
-      <c r="C19" s="5">
-        <v>2314</v>
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D19" s="5">
-        <v>234</v>
-      </c>
-      <c r="E19" s="20">
-        <v>234234</v>
-      </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="32">

</xml_diff>

<commit_message>
update in pr, with pr code
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CENPRI\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED8BFF-3438-4507-98A9-70936BE3333E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -83,16 +85,52 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>unit/s</t>
+  </si>
+  <si>
+    <t>Bacolod</t>
+  </si>
+  <si>
+    <t>Jonah</t>
+  </si>
+  <si>
+    <t>pr2019-1001</t>
+  </si>
+  <si>
+    <t>Test Purpose</t>
+  </si>
+  <si>
+    <t>Test Enduse</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
     <t xml:space="preserve">  Department:</t>
   </si>
   <si>
-    <t>(Y-m-d)</t>
+    <t>Dept. PR Code</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -272,12 +310,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,7 +322,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -293,16 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -318,12 +344,30 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,24 +380,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,15 +402,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -415,7 +444,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -709,11 +744,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:K19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,162 +772,179 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="41" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="42" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="43" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="40"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
       <c r="H7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="17">
+        <v>43656</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
       <c r="H8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="8"/>
+      <c r="I10" s="19">
+        <v>2</v>
+      </c>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
+      <c r="C11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="28" t="s">
+        <v>25</v>
+      </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -903,270 +955,152 @@
       <c r="K12" s="30"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="23" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="25" t="s">
+      <c r="I13" s="24"/>
+      <c r="J13" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="26"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>123</v>
-      </c>
-      <c r="B14" s="5">
-        <v>213</v>
-      </c>
-      <c r="C14" s="5">
-        <v>2314</v>
-      </c>
-      <c r="D14" s="5">
-        <v>2134</v>
-      </c>
-      <c r="E14" s="20">
-        <v>234</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>123</v>
-      </c>
-      <c r="B15" s="5">
-        <v>123</v>
-      </c>
-      <c r="C15" s="5">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5">
-        <v>34</v>
-      </c>
-      <c r="E15" s="20">
-        <v>234</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>213</v>
-      </c>
-      <c r="B16" s="5">
-        <v>213</v>
-      </c>
-      <c r="C16" s="5">
-        <v>24</v>
-      </c>
-      <c r="D16" s="5">
-        <v>234</v>
-      </c>
-      <c r="E16" s="20">
-        <v>324</v>
-      </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>213</v>
-      </c>
-      <c r="B17" s="5">
-        <v>213</v>
-      </c>
-      <c r="C17" s="5">
-        <v>324</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2134</v>
-      </c>
-      <c r="E17" s="20">
-        <v>234</v>
-      </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="24"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>123</v>
-      </c>
-      <c r="B18" s="5">
-        <v>23</v>
-      </c>
-      <c r="C18" s="5">
-        <v>2314</v>
-      </c>
-      <c r="D18" s="5">
-        <v>234</v>
-      </c>
-      <c r="E18" s="20">
-        <v>234</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>213</v>
-      </c>
-      <c r="B19" s="5">
-        <v>213</v>
-      </c>
-      <c r="C19" s="5">
-        <v>2314</v>
-      </c>
-      <c r="D19" s="5">
-        <v>234</v>
-      </c>
-      <c r="E19" s="20">
-        <v>234234</v>
-      </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+        <v>3</v>
+      </c>
+      <c r="B16" s="4">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
+  <mergeCells count="27">
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="J13:K13"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E13:I13"/>
     <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DE01D6-67CB-4BF6-BACE-F6E579A77432}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
POD Moved to PO
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CENPRI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED8BFF-3438-4507-98A9-70936BE3333E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -85,52 +83,16 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>unit/s</t>
-  </si>
-  <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>Jonah</t>
-  </si>
-  <si>
-    <t>pr2019-1001</t>
-  </si>
-  <si>
-    <t>Test Purpose</t>
-  </si>
-  <si>
-    <t>Test Enduse</t>
-  </si>
-  <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>Keyboard</t>
-  </si>
-  <si>
-    <t>Speakers</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Department:</t>
   </si>
   <si>
-    <t>Dept. PR Code</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Code</t>
+    <t>(Y-m-d)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -310,11 +272,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,6 +285,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -329,6 +293,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -344,6 +318,24 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,31 +345,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -387,21 +373,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -444,13 +415,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -744,11 +709,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,179 +737,162 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="31" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="10"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="33" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="10"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="35" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
       <c r="H7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="17">
-        <v>43656</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
       <c r="H8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
+        <v>5</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
       <c r="H9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="21"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="H10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="19">
-        <v>2</v>
-      </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>25</v>
-      </c>
+      <c r="C12" s="28"/>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -955,152 +903,270 @@
       <c r="K12" s="30"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="23" t="s">
+      <c r="I13" s="26"/>
+      <c r="J13" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="24"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+        <v>123</v>
+      </c>
+      <c r="B14" s="5">
+        <v>213</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2314</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2134</v>
+      </c>
+      <c r="E14" s="20">
+        <v>234</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
+        <v>123</v>
+      </c>
+      <c r="B15" s="5">
+        <v>123</v>
+      </c>
+      <c r="C15" s="5">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5">
+        <v>34</v>
+      </c>
+      <c r="E15" s="20">
+        <v>234</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
+        <v>213</v>
+      </c>
+      <c r="B16" s="5">
+        <v>213</v>
+      </c>
+      <c r="C16" s="5">
+        <v>24</v>
+      </c>
+      <c r="D16" s="5">
+        <v>234</v>
+      </c>
+      <c r="E16" s="20">
+        <v>324</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>213</v>
+      </c>
+      <c r="B17" s="5">
+        <v>213</v>
+      </c>
+      <c r="C17" s="5">
+        <v>324</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2134</v>
+      </c>
+      <c r="E17" s="20">
+        <v>234</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>123</v>
+      </c>
+      <c r="B18" s="5">
+        <v>23</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2314</v>
+      </c>
+      <c r="D18" s="5">
+        <v>234</v>
+      </c>
+      <c r="E18" s="20">
+        <v>234</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>213</v>
+      </c>
+      <c r="B19" s="5">
+        <v>213</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2314</v>
+      </c>
+      <c r="D19" s="5">
+        <v>234</v>
+      </c>
+      <c r="E19" s="20">
+        <v>234234</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="32">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:I13"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I10:K10"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DE01D6-67CB-4BF6-BACE-F6E579A77432}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add delete function in PR Group And create update function in signatories
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -2,18 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FLRJSN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -84,13 +83,13 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
-    <t>unit/s</t>
-  </si>
-  <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>pr2019-1001</t>
+    <t xml:space="preserve">  Department:</t>
+  </si>
+  <si>
+    <t>Test Purchase</t>
+  </si>
+  <si>
+    <t>PR2019-07-09</t>
   </si>
   <si>
     <t>Test Purpose</t>
@@ -99,43 +98,31 @@
     <t>Test Enduse</t>
   </si>
   <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>Keyboard</t>
-  </si>
-  <si>
-    <t>Speakers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Department:</t>
-  </si>
-  <si>
-    <t>Dept. PR Code</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Code</t>
+    <t>IT Department</t>
+  </si>
+  <si>
+    <t>Stephine</t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t xml:space="preserve">test </t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>Jason Flor</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>pin</t>
+    <t>Test Screw</t>
+  </si>
+  <si>
+    <t>Test Hammer</t>
+  </si>
+  <si>
+    <t>Test Ballpen</t>
+  </si>
+  <si>
+    <t>Test Pencil</t>
+  </si>
+  <si>
+    <t>Test Paper</t>
+  </si>
+  <si>
+    <t>Test Monitor</t>
   </si>
 </sst>
 </file>
@@ -321,11 +308,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -333,6 +321,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -340,78 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -421,7 +338,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,13 +441,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -767,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,400 +763,383 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="17" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="19" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="10"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="20" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="10"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="25" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="H7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="24"/>
+        <v>19</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="28"/>
       <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="21">
-        <v>43813</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="19">
+        <v>43655</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
       <c r="H8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+        <v>5</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
       <c r="H9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="24"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="27">
+        <v>2</v>
+      </c>
+      <c r="J9" s="28"/>
       <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="H10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="23">
-        <v>3</v>
-      </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="29"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="24"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="28"/>
       <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="37"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="31" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="32"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="41"/>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5">
+        <v>124</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="4">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="41"/>
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5">
+        <v>12354</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="4">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="38" t="s">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="15"/>
+      <c r="D16" s="5">
+        <v>1312354</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B17" s="16">
-        <v>2</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
+      <c r="B17" s="5">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="5">
+        <v>32146</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
-      <c r="B18" s="16">
-        <v>3</v>
-      </c>
-      <c r="C18" s="16" t="s">
+      <c r="B18" s="5">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="5">
+        <v>234</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="15"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="B19" s="16">
-        <v>5</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="38" t="s">
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="5">
         <v>36</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="15"/>
+      <c r="E19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I10:K10"/>
+  <mergeCells count="32">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates in displaying PO Summary
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CENPRI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED8BFF-3438-4507-98A9-70936BE3333E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -85,19 +83,13 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>unit/s</t>
-  </si>
-  <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>Jonah</t>
-  </si>
-  <si>
-    <t>pr2019-1001</t>
+    <t xml:space="preserve">  Department:</t>
+  </si>
+  <si>
+    <t>Test Purchase</t>
+  </si>
+  <si>
+    <t>PR2019-07-09</t>
   </si>
   <si>
     <t>Test Purpose</t>
@@ -106,31 +98,37 @@
     <t>Test Enduse</t>
   </si>
   <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>Keyboard</t>
-  </si>
-  <si>
-    <t>Speakers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Department:</t>
-  </si>
-  <si>
-    <t>Dept. PR Code</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Code</t>
+    <t>IT Department</t>
+  </si>
+  <si>
+    <t>Stephine</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Test Screw</t>
+  </si>
+  <si>
+    <t>Test Hammer</t>
+  </si>
+  <si>
+    <t>Test Ballpen</t>
+  </si>
+  <si>
+    <t>Test Pencil</t>
+  </si>
+  <si>
+    <t>Test Paper</t>
+  </si>
+  <si>
+    <t>Test Monitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -310,11 +308,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,6 +321,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -344,6 +344,24 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,31 +371,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -387,21 +399,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -444,13 +441,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -744,11 +735,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,335 +763,383 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="31" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="10"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="33" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="10"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="35" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="19">
+        <v>43655</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="H8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="27">
+        <v>2</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="H7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="17">
-        <v>43656</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="H8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="H9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="19" t="s">
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="21"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="19" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="H10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="19">
-        <v>2</v>
-      </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="23" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="24"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="14" t="s">
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+      <c r="D14" s="5">
+        <v>124</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="4">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5">
+        <v>12354</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="4">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1312354</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
         <v>20</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
+      <c r="C17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="5">
+        <v>32146</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="5">
+        <v>234</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="5">
+        <v>36</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="32">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:I13"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I10:K10"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E16:I16"/>
     <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DE01D6-67CB-4BF6-BACE-F6E579A77432}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add terms and condition in reporder and po_direct display and insert
</commit_message>
<xml_diff>
--- a/uploads/excel/Purchase Request.xlsx
+++ b/uploads/excel/Purchase Request.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -84,73 +84,175 @@
     <t xml:space="preserve">   Urgency No.:</t>
   </si>
   <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>Jonah</t>
-  </si>
-  <si>
-    <t>pr2019-1001</t>
-  </si>
-  <si>
-    <t>Test Purpose</t>
-  </si>
-  <si>
-    <t>Test Enduse</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Department:</t>
   </si>
   <si>
-    <t>Dept. PR Code</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
     <t>Code</t>
   </si>
   <si>
+    <t>HR - BCD</t>
+  </si>
+  <si>
+    <t>HRB</t>
+  </si>
+  <si>
+    <t>Billing Department</t>
+  </si>
+  <si>
+    <t>BIL</t>
+  </si>
+  <si>
+    <t>EIC</t>
+  </si>
+  <si>
+    <t>Environment/PCO</t>
+  </si>
+  <si>
+    <t>ENV</t>
+  </si>
+  <si>
+    <t>Finance Department</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>Fuel and Lube Management</t>
+  </si>
+  <si>
+    <t>FLM</t>
+  </si>
+  <si>
+    <t>Health and Safety</t>
+  </si>
+  <si>
+    <t>HAS</t>
+  </si>
+  <si>
+    <t>IT Department - BCD</t>
+  </si>
+  <si>
+    <t>ITB</t>
+  </si>
+  <si>
+    <t>IT Department - SITE</t>
+  </si>
+  <si>
+    <t>ITS</t>
+  </si>
+  <si>
+    <t>Laboratory and Chemical</t>
+  </si>
+  <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>MAI</t>
+  </si>
+  <si>
+    <t>Office of the GM</t>
+  </si>
+  <si>
+    <t>OOG</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>OPE</t>
+  </si>
+  <si>
+    <t>Purchasing Department</t>
+  </si>
+  <si>
+    <t>PUR</t>
+  </si>
+  <si>
+    <t>Reconditioning</t>
+  </si>
+  <si>
+    <t>REC</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>HR - SITE</t>
+  </si>
+  <si>
+    <t>HRS</t>
+  </si>
+  <si>
+    <t>Special Proj/Facilities Imp</t>
+  </si>
+  <si>
+    <t>SPE</t>
+  </si>
+  <si>
+    <t>Trading Department</t>
+  </si>
+  <si>
+    <t>TRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse - CENPRI </t>
+  </si>
+  <si>
+    <t>WHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse - Progen </t>
+  </si>
+  <si>
+    <t>WHP</t>
+  </si>
+  <si>
+    <t>Dept. Code</t>
+  </si>
+  <si>
+    <t>TEST PURCHASE</t>
+  </si>
+  <si>
+    <t>PR-IT</t>
+  </si>
+  <si>
+    <t>Stephine David Severino</t>
+  </si>
+  <si>
+    <t>TEST PURPOSE</t>
+  </si>
+  <si>
+    <t>TEST ENDUSE</t>
+  </si>
+  <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>mouse</t>
-  </si>
-  <si>
-    <t>keyboard</t>
-  </si>
-  <si>
-    <t>cpu</t>
-  </si>
-  <si>
-    <t>speaker</t>
-  </si>
-  <si>
-    <t>screw</t>
-  </si>
-  <si>
-    <t>cord</t>
-  </si>
-  <si>
-    <t>wire</t>
-  </si>
-  <si>
-    <t>monitor</t>
-  </si>
-  <si>
-    <t>a4 bond paper</t>
-  </si>
-  <si>
-    <t>earphone</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
+    <t>Test Mouse</t>
+  </si>
+  <si>
+    <t>Test Keyboard</t>
+  </si>
+  <si>
+    <t>Test Wifi Adapter</t>
+  </si>
+  <si>
+    <t>Test Monitor</t>
+  </si>
+  <si>
+    <t>Test CPU</t>
+  </si>
+  <si>
+    <t>Test Headset</t>
   </si>
 </sst>
 </file>
@@ -160,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +289,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,7 +465,73 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -366,72 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,7 +586,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -774,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,14 +913,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -818,14 +928,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -833,14 +943,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -848,140 +958,140 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="H7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
+      <c r="I7" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="18">
-        <v>43656</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="H8" s="3" t="s">
-        <v>25</v>
+      <c r="B8" s="20"/>
+      <c r="C8" s="26">
+        <v>43691</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="H8" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
+      <c r="I9" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
       <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="20">
-        <v>2</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
+      <c r="I10" s="29">
+        <v>1</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
+      <c r="C11" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="31"/>
+      <c r="C12" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -996,316 +1106,191 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="24" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="25"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18">
-        <v>43517</v>
-      </c>
-      <c r="K14" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="4">
+        <v>123</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>5</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="18">
-        <v>43518</v>
-      </c>
-      <c r="K15" s="19"/>
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1222</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="14">
-        <v>10</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="18">
-        <v>43519</v>
-      </c>
-      <c r="K16" s="19"/>
+      <c r="B16" s="4">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="4">
+        <v>13421</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B17" s="14">
-        <v>3</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18">
-        <v>43520</v>
-      </c>
-      <c r="K17" s="19"/>
+      <c r="B17" s="4">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="4">
+        <v>14543</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="28"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
-      <c r="B18" s="14">
-        <v>4</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18">
-        <v>43521</v>
-      </c>
-      <c r="K18" s="19"/>
+      <c r="B18" s="4">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="4">
+        <v>12424</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>5</v>
-      </c>
-      <c r="B19" s="14">
-        <v>4</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="18">
-        <v>43522</v>
-      </c>
-      <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>5</v>
-      </c>
-      <c r="B20" s="14">
-        <v>4</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="18">
-        <v>43523</v>
-      </c>
-      <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>5</v>
-      </c>
-      <c r="B21" s="14">
-        <v>4</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18">
-        <v>43524</v>
-      </c>
-      <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>5</v>
-      </c>
-      <c r="B22" s="14">
-        <v>4</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18">
-        <v>43525</v>
-      </c>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>5</v>
-      </c>
-      <c r="B23" s="14">
-        <v>4</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18">
-        <v>43526</v>
-      </c>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>5</v>
-      </c>
-      <c r="B24" s="14">
-        <v>4</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="18">
-        <v>43527</v>
-      </c>
-      <c r="K24" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="B19" s="4">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2134</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="E16:I16"/>
+  <mergeCells count="33">
     <mergeCell ref="E17:I17"/>
     <mergeCell ref="E18:I18"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E19:I19"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1315,27 +1300,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>